<commit_message>
playing with multiple variable models: does coral cover, bleaching, disease, and paling influence the hog fish abundance? game fish abundance?
</commit_message>
<xml_diff>
--- a/TEST_2018_bisc_coral_health_data.xlsx
+++ b/TEST_2018_bisc_coral_health_data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3490" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3490" uniqueCount="71">
   <si>
     <t>JV</t>
   </si>
@@ -234,6 +234,9 @@
   </si>
   <si>
     <t>coral_species</t>
+  </si>
+  <si>
+    <t>site</t>
   </si>
 </sst>
 </file>
@@ -948,7 +951,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A449" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F189" sqref="F189"/>
+      <selection pane="bottomLeft" activeCell="C458" sqref="C458"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -958,7 +961,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>70</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>

</xml_diff>